<commit_message>
Ticket #9517 cal sheet corrections and updates by Steve Gaul for Pioneer ADCP.
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP02PMUO_00002.xlsx
+++ b/deployment/Omaha_Cal_Info_CP02PMUO_00002.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\CP_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Desktop\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8952" yWindow="9408" windowWidth="20736" windowHeight="9888" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14064" windowHeight="8436" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="84">
   <si>
     <t>Ref Des</t>
   </si>
@@ -310,9 +310,6 @@
     </r>
   </si>
   <si>
-    <t>CP02PMUO-MOPAK</t>
-  </si>
-  <si>
     <t>Mooring OOIBARCODE</t>
   </si>
   <si>
@@ -344,6 +341,18 @@
   </si>
   <si>
     <t>43-2499</t>
+  </si>
+  <si>
+    <t>A00069</t>
+  </si>
+  <si>
+    <t>CP02PMUO-00002-MOPAK</t>
+  </si>
+  <si>
+    <t>R00008</t>
+  </si>
+  <si>
+    <t>R00009</t>
   </si>
 </sst>
 </file>
@@ -466,7 +475,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -488,6 +497,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,7 +554,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -582,9 +597,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -608,6 +620,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1005,46 +1023,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="25" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>11</v>
@@ -1064,10 +1082,10 @@
       <c r="G2" s="5">
         <v>41743</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>65</v>
       </c>
       <c r="J2" s="2">
@@ -1077,18 +1095,18 @@
         <v>13</v>
       </c>
       <c r="L2" s="6"/>
-      <c r="M2" s="25">
+      <c r="M2" s="24">
         <f>((LEFT(H2,(FIND("°",H2,1)-1)))+(MID(H2,(FIND("°",H2,1)+1),(FIND("'",H2,1))-(FIND("°",H2,1)+1))/60))*(IF(RIGHT(H2,1)="N",1,-1))</f>
         <v>39.937983333333335</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="24">
         <f>((LEFT(I2,(FIND("°",I2,1)-1)))+(MID(I2,(FIND("°",I2,1)+1),(FIND("'",I2,1))-(FIND("°",I2,1)+1))/60))*(IF(RIGHT(I2,1)="E",1,-1))</f>
         <v>-70.769083333333327</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1105,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1116,7 +1134,7 @@
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47" customWidth="1"/>
     <col min="8" max="8" width="20.109375" customWidth="1"/>
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
@@ -1127,7 +1145,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
@@ -1136,7 +1154,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>15</v>
@@ -1153,7 +1171,7 @@
         <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>12</v>
@@ -1161,8 +1179,8 @@
       <c r="D2" s="8">
         <v>2</v>
       </c>
-      <c r="E2" s="17">
-        <v>18445</v>
+      <c r="E2" s="26" t="s">
+        <v>80</v>
       </c>
       <c r="F2" s="8">
         <v>18445</v>
@@ -1170,10 +1188,10 @@
       <c r="G2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="22">
+      <c r="H2" s="21">
         <v>430000</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>66</v>
       </c>
       <c r="J2" s="7"/>
@@ -1185,7 +1203,7 @@
         <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>12</v>
@@ -1193,8 +1211,8 @@
       <c r="D3" s="8">
         <v>2</v>
       </c>
-      <c r="E3" s="17">
-        <v>18445</v>
+      <c r="E3" s="26" t="s">
+        <v>80</v>
       </c>
       <c r="F3" s="8">
         <v>18445</v>
@@ -1215,7 +1233,7 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
@@ -1223,8 +1241,8 @@
       <c r="D4" s="8">
         <v>2</v>
       </c>
-      <c r="E4" s="17">
-        <v>18445</v>
+      <c r="E4" s="26" t="s">
+        <v>80</v>
       </c>
       <c r="F4" s="8">
         <v>18445</v>
@@ -1245,7 +1263,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="17"/>
+      <c r="E5" s="16"/>
       <c r="F5" s="8"/>
       <c r="G5" s="7"/>
       <c r="H5" s="9"/>
@@ -1259,7 +1277,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>12</v>
@@ -1267,13 +1285,15 @@
       <c r="D6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="16" t="s">
-        <v>69</v>
+      <c r="E6" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="17" t="s">
         <v>61</v>
       </c>
       <c r="J6" s="7"/>
@@ -1285,7 +1305,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>12</v>
@@ -1294,10 +1314,10 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
         <v>79</v>
-      </c>
-      <c r="F8" t="s">
-        <v>80</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>22</v>
@@ -1317,7 +1337,7 @@
         <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>12</v>
@@ -1326,10 +1346,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s">
         <v>79</v>
-      </c>
-      <c r="F9" t="s">
-        <v>80</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>19</v>
@@ -1347,7 +1367,7 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>12</v>
@@ -1356,10 +1376,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
         <v>79</v>
-      </c>
-      <c r="F10" t="s">
-        <v>80</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>20</v>
@@ -1377,7 +1397,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>12</v>
@@ -1386,10 +1406,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" t="s">
         <v>79</v>
-      </c>
-      <c r="F11" t="s">
-        <v>80</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>24</v>
@@ -1409,7 +1429,7 @@
         <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>12</v>
@@ -1418,10 +1438,10 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" t="s">
         <v>79</v>
-      </c>
-      <c r="F12" t="s">
-        <v>80</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>26</v>
@@ -1441,7 +1461,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>12</v>
@@ -1450,10 +1470,10 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s">
         <v>79</v>
-      </c>
-      <c r="F13" t="s">
-        <v>80</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>28</v>
@@ -1473,7 +1493,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>12</v>
@@ -1482,10 +1502,10 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F14" t="s">
         <v>79</v>
-      </c>
-      <c r="F14" t="s">
-        <v>80</v>
       </c>
       <c r="G14" s="7" t="s">
         <v>30</v>
@@ -1505,7 +1525,7 @@
         <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>12</v>
@@ -1514,10 +1534,10 @@
         <v>2</v>
       </c>
       <c r="E15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" t="s">
         <v>79</v>
-      </c>
-      <c r="F15" t="s">
-        <v>80</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>32</v>
@@ -1550,7 +1570,7 @@
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>12</v>
@@ -1559,7 +1579,7 @@
         <v>2</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F17" s="8">
         <v>113</v>
@@ -1580,7 +1600,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>12</v>
@@ -1589,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F18" s="8">
         <v>113</v>
@@ -1610,7 +1630,7 @@
       <c r="B19" s="7"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="17"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
       <c r="H19" s="9"/>
@@ -1624,7 +1644,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>12</v>
@@ -1633,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F20" s="11">
         <v>100013</v>
@@ -1654,7 +1674,7 @@
         <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>12</v>
@@ -1663,7 +1683,7 @@
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F21" s="11">
         <v>100013</v>
@@ -1684,7 +1704,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="17"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="11"/>
       <c r="G22" s="7"/>
       <c r="H22" s="9"/>
@@ -1698,7 +1718,7 @@
         <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>12</v>
@@ -1707,7 +1727,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" s="8">
         <v>1031</v>
@@ -1715,7 +1735,7 @@
       <c r="G23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="22">
         <v>1.0760000000000001</v>
       </c>
       <c r="I23" s="8" t="s">
@@ -1730,7 +1750,7 @@
         <v>38</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>12</v>
@@ -1739,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F24" s="8">
         <v>1031</v>
@@ -1762,7 +1782,7 @@
         <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>12</v>
@@ -1771,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F25" s="8">
         <v>1031</v>
@@ -1794,7 +1814,7 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>12</v>
@@ -1803,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F26" s="8">
         <v>1031</v>
@@ -1826,7 +1846,7 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>12</v>
@@ -1835,7 +1855,7 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F27" s="8">
         <v>1031</v>
@@ -1843,7 +1863,7 @@
       <c r="G27" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="22">
         <v>3.9E-2</v>
       </c>
       <c r="I27" s="8" t="s">
@@ -1858,7 +1878,7 @@
         <v>38</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
@@ -1867,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F28" s="8">
         <v>1031</v>
@@ -1875,7 +1895,7 @@
       <c r="G28" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="22">
         <v>700</v>
       </c>
       <c r="I28" s="8" t="s">
@@ -1890,7 +1910,7 @@
         <v>38</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>12</v>
@@ -1899,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F29" s="8">
         <v>1031</v>
@@ -1922,7 +1942,7 @@
         <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>12</v>
@@ -1931,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F30" s="8">
         <v>1031</v>
@@ -1954,7 +1974,7 @@
         <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>12</v>
@@ -1963,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="8">
         <v>1031</v>
@@ -1986,7 +2006,7 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>12</v>
@@ -1995,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32" s="8">
         <v>1031</v>
@@ -2003,7 +2023,7 @@
       <c r="G32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="22">
         <v>124</v>
       </c>
       <c r="I32" s="8" t="s">
@@ -2018,7 +2038,7 @@
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="17"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="8"/>
       <c r="G33" s="7"/>
       <c r="H33" s="9"/>
@@ -2032,7 +2052,7 @@
         <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>12</v>
@@ -2041,7 +2061,7 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34">
         <v>20477</v>
@@ -2064,7 +2084,7 @@
         <v>55</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>12</v>
@@ -2073,7 +2093,7 @@
         <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35">
         <v>20477</v>
@@ -2110,19 +2130,19 @@
         <v>62</v>
       </c>
       <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" s="8">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" t="s">
         <v>72</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D37" s="8">
-        <v>2</v>
-      </c>
-      <c r="E37" t="s">
-        <v>75</v>
-      </c>
-      <c r="F37" t="s">
-        <v>73</v>
       </c>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
@@ -2136,7 +2156,7 @@
         <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>12</v>
@@ -2144,13 +2164,15 @@
       <c r="D39" s="8">
         <v>2</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="24" t="s">
+      <c r="E39" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="23" t="s">
         <v>67</v>
       </c>
       <c r="G39" s="7"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="18"/>
+      <c r="H39" s="16"/>
+      <c r="I39" s="17"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
@@ -2160,11 +2182,11 @@
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
-      <c r="E40" s="17"/>
+      <c r="E40" s="16"/>
       <c r="F40" s="8"/>
       <c r="G40" s="7"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="18"/>
+      <c r="I40" s="17"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
       <c r="L40" s="7"/>

</xml_diff>